<commit_message>
ajuste para fazer os mesmos testes para os algoritmos.
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,26 +474,86 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[2, 5, 4]</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.166666666666667</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.0001971721649169922</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[3]</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7.05718994140625e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[9]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[1]</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0001795291900634766</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.319450378417969e-05</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -508,7 +568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,26 +625,86 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>11</v>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[4, 1, 2, 3, 6, 5, 8, 7, 10, 11]</t>
+          <t>[2, 3, 6, 5, 4]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8.130073547363281e-05</v>
+        <v>7.939338684082031e-05</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[3]</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0001015663146972656</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[9]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9.512901306152344e-05</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -599,7 +719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -656,26 +776,86 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[5]</t>
+          <t>[2, 5, 4]</t>
         </is>
       </c>
       <c r="E2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9.799003601074219e-05</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[3]</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0001027584075927734</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6.723403930664062e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[9]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.365776062011719e-05</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -690,7 +870,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -747,26 +927,86 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[2, 5, 4]</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>3</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>[3, 2]</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>2</v>
       </c>
       <c r="F2" t="n">
         <v>2.692307692307693</v>
       </c>
       <c r="G2" t="n">
-        <v>0.000232696533203125</v>
+        <v>0.0001680850982666016</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[3]</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.692307692307693</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7.367134094238281e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[9]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.692307692307693</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.104873657226562e-05</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -781,7 +1021,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -838,26 +1078,86 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[6, 5, 8, 7]</t>
+          <t>[2, 5, 4]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
         <v>2.692307692307693</v>
       </c>
       <c r="G2" t="n">
-        <v>0.001755714416503906</v>
+        <v>0.006186723709106445</v>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[3]</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.692307692307693</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.153915405273438e-05</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[9]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.692307692307693</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0001342296600341797</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajuste no formato das coordenadas e mapeado os pontos do 14 ao 32
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -474,24 +474,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[2, 5, 4]</t>
+          <t>[4, 5]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>1.166666666666667</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001971721649169922</v>
+        <v>0.000301361083984375</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -507,21 +507,21 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 6, 9, 13, 17, 20, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1.037037037037037</v>
       </c>
       <c r="G3" t="n">
-        <v>7.05718994140625e-05</v>
+        <v>0.000102996826171875</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -534,24 +534,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[11, 12, 13, 17, 20]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1.136363636363636</v>
       </c>
       <c r="G4" t="n">
-        <v>7.319450378417969e-05</v>
+        <v>8.034706115722656e-05</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -625,14 +625,14 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[2, 3, 6, 5, 4]</t>
+          <t>[4, 1, 2, 3, 6, 5]</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>7.939338684082031e-05</v>
+        <v>0.0001111030578613281</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -658,21 +658,21 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 2, 5, 4, 7, 8, 9, 6, 27, 28, 29, 13, 12, 11, 10, 14, 15, 16, 17, 20, 19, 18, 21, 22, 23, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.03448275862068965</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001015663146972656</v>
+        <v>7.557868957519531e-05</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -685,24 +685,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[11, 10, 7, 4, 1, 2, 3, 6, 5, 8, 9, 28, 29, 13, 12, 16, 15, 14, 18, 19, 20]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="G4" t="n">
-        <v>9.512901306152344e-05</v>
+        <v>7.605552673339844e-05</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -776,24 +776,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[2, 5, 4]</t>
+          <t>[4, 5]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="G2" t="n">
-        <v>9.799003601074219e-05</v>
+        <v>8.20159912109375e-05</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -809,21 +809,21 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 25, 26, 27, 28, 29, 13, 17, 20, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>0.6285714285714286</v>
       </c>
       <c r="G3" t="n">
-        <v>6.723403930664062e-05</v>
+        <v>9.298324584960938e-05</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -836,24 +836,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[11, 15, 16, 17, 20]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="G4" t="n">
-        <v>6.365776062011719e-05</v>
+        <v>7.653236389160156e-05</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -927,24 +927,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[2, 5, 4]</t>
+          <t>[4, 5]</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>2.692307692307693</v>
+        <v>3.0625</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001680850982666016</v>
+        <v>9.417533874511719e-05</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -960,21 +960,21 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 25, 26, 27, 28, 29, 30, 31, 20, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>2.692307692307693</v>
+        <v>3.0625</v>
       </c>
       <c r="G3" t="n">
-        <v>7.367134094238281e-05</v>
+        <v>9.5367431640625e-05</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -987,24 +987,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[11, 15, 16, 17, 20]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>2.692307692307693</v>
+        <v>3.0625</v>
       </c>
       <c r="G4" t="n">
-        <v>7.104873657226562e-05</v>
+        <v>0.000110626220703125</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -1078,24 +1078,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[2, 5, 4]</t>
+          <t>[4, 5]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F2" t="n">
-        <v>2.692307692307693</v>
+        <v>3.0625</v>
       </c>
       <c r="G2" t="n">
-        <v>0.006186723709106445</v>
+        <v>0.0002543926239013672</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1111,21 +1111,21 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[3, 25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>2.692307692307693</v>
+        <v>3.0625</v>
       </c>
       <c r="G3" t="n">
-        <v>8.153915405273438e-05</v>
+        <v>0.0001401901245117188</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -1138,24 +1138,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[9]</t>
+          <t>[11, 15, 16, 19, 20]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>2.692307692307693</v>
+        <v>3.0625</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001342296600341797</v>
+        <v>0.0001769065856933594</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
add novo pedaço do mama mapeado e organizando os testes.
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,24 +474,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[4, 5]</t>
+          <t>[13, 9, 8, 7]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F2" t="n">
-        <v>1.333333333333333</v>
+        <v>1.5</v>
       </c>
       <c r="G2" t="n">
-        <v>0.000301361083984375</v>
+        <v>0.0002608299255371094</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -504,24 +504,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3, 6, 9, 13, 17, 20, 24]</t>
+          <t>[30, 17, 20, 24, 23]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F3" t="n">
-        <v>1.037037037037037</v>
+        <v>1.238095238095238</v>
       </c>
       <c r="G3" t="n">
-        <v>0.000102996826171875</v>
+        <v>0.000125885009765625</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -534,26 +534,86 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[11, 12, 13, 17, 20]</t>
+          <t>[12, 8, 5, 6, 27, 26]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F4" t="n">
-        <v>1.136363636363636</v>
+        <v>1.068965517241379</v>
       </c>
       <c r="G4" t="n">
-        <v>8.034706115722656e-05</v>
+        <v>9.179115295410156e-05</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[8, 7, 10, 14, 18]</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>24</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.041666666666667</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.821487426757812e-05</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[23, 19, 16, 12, 8, 5, 4]</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.867813110351562e-05</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -568,7 +628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,24 +685,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[4, 1, 2, 3, 6, 5]</t>
+          <t>[13, 9, 6, 3, 2, 5, 4, 7]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001111030578613281</v>
+        <v>7.390975952148438e-05</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -655,24 +715,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3, 2, 5, 4, 7, 8, 9, 6, 27, 28, 29, 13, 12, 11, 10, 14, 15, 16, 17, 20, 19, 18, 21, 22, 23, 24]</t>
+          <t>[30, 17, 13, 9, 6, 3, 2, 5, 4, 7, 8, 12, 11, 10, 14, 15, 16, 19, 18, 21, 22, 23]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03448275862068965</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>7.557868957519531e-05</v>
+        <v>6.890296936035156e-05</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -685,26 +745,86 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" t="n">
+        <v>26</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[12, 8, 5, 2, 3, 6, 9, 28, 27, 26]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>11</v>
       </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>[11, 10, 7, 4, 1, 2, 3, 6, 5, 8, 9, 28, 29, 13, 12, 16, 15, 14, 18, 19, 20]</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6.771087646484375e-05</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[8, 5, 2, 3, 6, 9, 28, 29, 13, 12, 11, 10, 14, 15, 16, 17, 20, 19, 18]</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7.486343383789062e-05</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[23, 19, 16, 12, 8, 5, 4]</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>24</v>
       </c>
-      <c r="F4" t="n">
-        <v>0.08333333333333333</v>
-      </c>
-      <c r="G4" t="n">
-        <v>7.605552673339844e-05</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="F6" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9.202957153320312e-05</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -719,7 +839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -776,24 +896,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[4, 5]</t>
+          <t>[13, 9, 8, 7]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="G2" t="n">
-        <v>8.20159912109375e-05</v>
+        <v>0.0001370906829833984</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -806,24 +926,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3, 25, 26, 27, 28, 29, 13, 17, 20, 24]</t>
+          <t>[30, 31, 32, 24, 23]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6285714285714286</v>
+        <v>0.7272727272727273</v>
       </c>
       <c r="G3" t="n">
-        <v>9.298324584960938e-05</v>
+        <v>8.96453857421875e-05</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -836,26 +956,86 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[11, 15, 16, 17, 20]</t>
+          <t>[12, 8, 5, 6, 27, 26]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5263157894736842</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="G4" t="n">
-        <v>7.653236389160156e-05</v>
+        <v>9.5367431640625e-05</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[8, 7, 10, 14, 18]</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>27</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9285714285714286</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9.441375732421875e-05</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[23, 22, 21, 18, 14, 10, 7, 4]</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>28</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9.34600830078125e-05</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -870,7 +1050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -927,24 +1107,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[4, 5]</t>
+          <t>[13, 9, 8, 7]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>3.0625</v>
       </c>
       <c r="G2" t="n">
-        <v>9.417533874511719e-05</v>
+        <v>0.0002100467681884766</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -957,24 +1137,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3, 25, 26, 27, 28, 29, 30, 31, 20, 24]</t>
+          <t>[30, 31, 32, 24, 23]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
         <v>3.0625</v>
       </c>
       <c r="G3" t="n">
-        <v>9.5367431640625e-05</v>
+        <v>0.0001180171966552734</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -987,26 +1167,86 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[11, 15, 16, 17, 20]</t>
+          <t>[12, 8, 5, 6, 27, 26]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F4" t="n">
         <v>3.0625</v>
       </c>
       <c r="G4" t="n">
-        <v>0.000110626220703125</v>
+        <v>0.0001308917999267578</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[8, 7, 10, 14, 18]</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>24</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0625</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.000118255615234375</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[23, 22, 21, 18, 14, 10, 7, 4]</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0625</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0001130104064941406</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1021,7 +1261,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,24 +1318,24 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[4, 5]</t>
+          <t>[13, 9, 8, 7]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>3.0625</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0002543926239013672</v>
+        <v>0.00026702880859375</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -1108,24 +1348,24 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[3, 25, 26, 27, 28, 29, 30, 31, 32, 24]</t>
+          <t>[30, 31, 32, 24, 23]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F3" t="n">
         <v>3.0625</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001401901245117188</v>
+        <v>0.0001494884490966797</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -1138,26 +1378,86 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[11, 15, 16, 19, 20]</t>
+          <t>[12, 8, 5, 6, 27, 26]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F4" t="n">
         <v>3.0625</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0001769065856933594</v>
+        <v>0.0001566410064697266</v>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>[8, 7, 10, 14, 18]</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3.0625</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0001356601715087891</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>23</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>[23, 22, 21, 18, 14, 10, 7, 4]</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>24</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.0625</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0001313686370849609</v>
+      </c>
+      <c r="H6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionada distancia total em metros no A_estrela e passada para a tabela.
</commit_message>
<xml_diff>
--- a/Relatório.xlsx
+++ b/Relatório.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,20 +448,25 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Distancia</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Quantidade de nós expandidos</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Fator de ramificação médio</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Memória Alocada</t>
         </is>
@@ -474,26 +479,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[13, 9, 8, 7]</t>
+          <t>[19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0002608299255371094</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0.000213623046875</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -504,26 +512,29 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[30, 17, 20, 24, 23]</t>
+          <t>[6, 9, 13]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.238095238095238</v>
+        <v>11</v>
       </c>
       <c r="G3" t="n">
-        <v>0.000125885009765625</v>
+        <v>1.363636363636364</v>
       </c>
       <c r="H3" t="n">
+        <v>0.0001287460327148438</v>
+      </c>
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -534,26 +545,29 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" t="n">
+        <v>31</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>[17, 20, 31]</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
         <v>12</v>
       </c>
-      <c r="C4" t="n">
-        <v>26</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>[12, 8, 5, 6, 27, 26]</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>29</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1.068965517241379</v>
-      </c>
       <c r="G4" t="n">
-        <v>9.179115295410156e-05</v>
+        <v>1.583333333333333</v>
       </c>
       <c r="H4" t="n">
+        <v>0.0001022815704345703</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -564,26 +578,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[8, 7, 10, 14, 18]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1.041666666666667</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>8.821487426757812e-05</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>7.867813110351562e-05</v>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -594,26 +611,29 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[23, 19, 16, 12, 8, 5, 4]</t>
+          <t>[3, 2, 5, 8, 12]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1.12</v>
+        <v>15</v>
       </c>
       <c r="G6" t="n">
-        <v>7.867813110351562e-05</v>
+        <v>1.133333333333333</v>
       </c>
       <c r="H6" t="n">
+        <v>8.821487426757812e-05</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -628,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,20 +679,25 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Distancia</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Quantidade de nós expandidos</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Fator de ramificação médio</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Memória Alocada</t>
         </is>
@@ -685,26 +710,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[13, 9, 6, 3, 2, 5, 4, 7]</t>
+          <t>[19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>7.390975952148438e-05</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>8.20159912109375e-05</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -715,26 +743,29 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[30, 17, 13, 9, 6, 3, 2, 5, 4, 7, 8, 12, 11, 10, 14, 15, 16, 19, 18, 21, 22, 23]</t>
+          <t>[6, 3, 2, 5, 4, 7, 8, 9, 28, 29, 13]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G3" t="n">
-        <v>6.890296936035156e-05</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="H3" t="n">
+        <v>7.796287536621094e-05</v>
+      </c>
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -745,26 +776,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[12, 8, 5, 2, 3, 6, 9, 28, 27, 26]</t>
+          <t>[17, 13, 9, 6, 3, 2, 5, 4, 7, 8, 12, 11, 10, 14, 15, 16, 19, 18, 21, 22, 23, 24, 20, 31]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G4" t="n">
-        <v>6.771087646484375e-05</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
+        <v>8.344650268554688e-05</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -775,26 +809,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[8, 5, 2, 3, 6, 9, 28, 29, 13, 12, 11, 10, 14, 15, 16, 17, 20, 19, 18]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.12</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>7.486343383789062e-05</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>7.128715515136719e-05</v>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -805,26 +842,29 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[23, 19, 16, 12, 8, 5, 4]</t>
+          <t>[3, 2, 5, 4, 7, 8, 9, 6, 27, 28, 29, 13, 12]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6666666666666666</v>
+        <v>16</v>
       </c>
       <c r="G6" t="n">
-        <v>9.202957153320312e-05</v>
+        <v>0.0625</v>
       </c>
       <c r="H6" t="n">
+        <v>7.414817810058594e-05</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -839,7 +879,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,20 +910,25 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Distancia</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Quantidade de nós expandidos</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Fator de ramificação médio</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Memória Alocada</t>
         </is>
@@ -896,26 +941,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[13, 9, 8, 7]</t>
+          <t>[19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8181818181818182</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0001370906829833984</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
+        <v>0.0001046657562255859</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -926,26 +974,29 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[30, 31, 32, 24, 23]</t>
+          <t>[6, 9, 13]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7272727272727273</v>
+        <v>9</v>
       </c>
       <c r="G3" t="n">
-        <v>8.96453857421875e-05</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="H3" t="n">
+        <v>0.0002241134643554688</v>
+      </c>
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -956,26 +1007,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[12, 8, 5, 6, 27, 26]</t>
+          <t>[17, 30, 31]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8888888888888888</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
-        <v>9.5367431640625e-05</v>
+        <v>0.4</v>
       </c>
       <c r="H4" t="n">
+        <v>0.0001020431518554688</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -986,26 +1040,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[8, 7, 10, 14, 18]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9285714285714286</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>9.441375732421875e-05</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
+        <v>0.0001242160797119141</v>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1016,26 +1073,29 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[23, 22, 21, 18, 14, 10, 7, 4]</t>
+          <t>[3, 6, 5, 8, 12]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9</v>
+        <v>18</v>
       </c>
       <c r="G6" t="n">
-        <v>9.34600830078125e-05</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="H6" t="n">
+        <v>0.0001125335693359375</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1050,7 +1110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1081,20 +1141,25 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Distancia</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Quantidade de nós expandidos</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Fator de ramificação médio</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Memória Alocada</t>
         </is>
@@ -1107,26 +1172,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[13, 9, 8, 7]</t>
+          <t>[19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.0002100467681884766</v>
-      </c>
       <c r="H2" t="n">
+        <v>0.0001130104064941406</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1137,26 +1205,29 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[30, 31, 32, 24, 23]</t>
+          <t>[6, 9, 13]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.0001180171966552734</v>
-      </c>
       <c r="H3" t="n">
+        <v>0.0001275539398193359</v>
+      </c>
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1167,26 +1238,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[12, 8, 5, 6, 27, 26]</t>
+          <t>[17, 30, 31]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.0001308917999267578</v>
-      </c>
       <c r="H4" t="n">
+        <v>0.0001168251037597656</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1197,26 +1271,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[8, 7, 10, 14, 18]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.000118255615234375</v>
-      </c>
       <c r="H5" t="n">
+        <v>0.0001053810119628906</v>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1227,26 +1304,29 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[23, 22, 21, 18, 14, 10, 7, 4]</t>
+          <t>[3, 6, 5, 8, 12]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>349</v>
       </c>
       <c r="F6" t="n">
+        <v>16</v>
+      </c>
+      <c r="G6" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.0001130104064941406</v>
-      </c>
       <c r="H6" t="n">
+        <v>0.0004928112030029297</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1261,7 +1341,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1292,20 +1372,25 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>Distancia</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Quantidade de nós expandidos</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Fator de ramificação médio</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Memória Alocada</t>
         </is>
@@ -1318,26 +1403,29 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>[13, 9, 8, 7]</t>
+          <t>[19]</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.00026702880859375</v>
-      </c>
       <c r="H2" t="n">
+        <v>0.003904104232788086</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1348,26 +1436,29 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>[30, 31, 32, 24, 23]</t>
+          <t>[6, 9, 13]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="F3" t="n">
+        <v>9</v>
+      </c>
+      <c r="G3" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.0001494884490966797</v>
-      </c>
       <c r="H3" t="n">
+        <v>0.0001533031463623047</v>
+      </c>
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1378,26 +1469,29 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>[12, 8, 5, 6, 27, 26]</t>
+          <t>[17, 30, 31]</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="F4" t="n">
+        <v>6</v>
+      </c>
+      <c r="G4" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G4" t="n">
-        <v>0.0001566410064697266</v>
-      </c>
       <c r="H4" t="n">
+        <v>0.0001726150512695312</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1408,26 +1502,29 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>[8, 7, 10, 14, 18]</t>
+          <t>[14]</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G5" t="n">
-        <v>0.0001356601715087891</v>
-      </c>
       <c r="H5" t="n">
+        <v>0.0001351833343505859</v>
+      </c>
+      <c r="I5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1438,26 +1535,29 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[23, 22, 21, 18, 14, 10, 7, 4]</t>
+          <t>[3, 6, 5, 8, 12]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>24</v>
+        <v>349</v>
       </c>
       <c r="F6" t="n">
+        <v>16</v>
+      </c>
+      <c r="G6" t="n">
         <v>3.0625</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.0001313686370849609</v>
-      </c>
       <c r="H6" t="n">
+        <v>0.0001521110534667969</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>